<commit_message>
SSL bug fix, console messages update
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1409,7 +1409,2457 @@
           <t xml:space="preserve"> - ?? </t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>https://www.iol.pt</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>https://www.observador.pt</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>https://www.elcorteingles.pt</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>https://www.expresso.pt</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>https://www.rtp.pt</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Escolhe esta opção apenas nos teus dispositivos pessoais para manter a tua conta segura.                Iniciar sessão  Já tem uma conta?      Ainda não tem conta? Inscreva-se gratuitamente    Repor a sua palavra-passe  r       Introduza o seu e-mail para receber as instruções para recuperar a palavra-passe:                  Enviar-me as instruções        O e-mail foi enviado para  Siga as instruções no e-mail para repor a sua palavra-passe. Se não receber oe-mail na sua caixa de entrada, consulte a pasta de spam. O remetente énoreply@edreams.com.     \  Voltar a Iniciar sessão            Ative o Javascript  Para que este site funcione corretamente, tem de ativar o JavaScript</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>https://www.cmjornal.pt</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>https://www.jornaldenegocios.pt</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>https://www.telepizza.pt</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>gricrp.cc@sef.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>https://www.linguee.pt</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>http://www.idealista.pt</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>https://www.legendasdivx.pt</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">									Ligue 210 988 616 | 963 828 885 ou envie-nos um e-mail para: geral@atesempre.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>https://www.jn.pt</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>https://www.ulisboa.pt</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>http://www.acesso.gov.pt</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>E reitoria@ulisboa.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>https://www.ipl.pt</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>https://www.jogossantacasa.pt</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>https://www.lidl.pt</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>https://www.rostos.pt</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>https://www.betclic.pt</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>https://www.iol.pt</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>https://www.observador.pt</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>https://www.elcorteingles.pt</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>https://www.expresso.pt</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>https://www.rtp.pt</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Escolhe esta opção apenas nos teus dispositivos pessoais para manter a tua conta segura.                Iniciar sessão  Já tem uma conta?      Ainda não tem conta? Inscreva-se gratuitamente    Repor a sua palavra-passe  r       Introduza o seu e-mail para receber as instruções para recuperar a palavra-passe:                  Enviar-me as instruções        O e-mail foi enviado para  Siga as instruções no e-mail para repor a sua palavra-passe. Se não receber oe-mail na sua caixa de entrada, consulte a pasta de spam. O remetente énoreply@edreams.com.     \  Voltar a Iniciar sessão            Ative o Javascript  Para que este site funcione corretamente, tem de ativar o JavaScript</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>https://www.cmjornal.pt</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>https://www.jornaldenegocios.pt</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>https://www.telepizza.pt</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>gricrp.cc@sef.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>https://www.linguee.pt</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>http://www.idealista.pt</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>https://www.legendasdivx.pt</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">									Ligue 210 988 616 | 963 828 885 ou envie-nos um e-mail para: geral@atesempre.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>https://www.jn.pt</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>https://www.ulisboa.pt</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>http://www.acesso.gov.pt</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>E reitoria@ulisboa.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>https://www.ipl.pt</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>https://www.jogossantacasa.pt</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>https://www.lidl.pt</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>https://www.rostos.pt</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>https://www.betclic.pt</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>https://www.iol.pt</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>https://www.observador.pt</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>https://www.elcorteingles.pt</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>https://www.expresso.pt</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>https://www.rtp.pt</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Escolhe esta opção apenas nos teus dispositivos pessoais para manter a tua conta segura.                Iniciar sessão  Já tem uma conta?      Ainda não tem conta? Inscreva-se gratuitamente    Repor a sua palavra-passe  r       Introduza o seu e-mail para receber as instruções para recuperar a palavra-passe:                  Enviar-me as instruções        O e-mail foi enviado para  Siga as instruções no e-mail para repor a sua palavra-passe. Se não receber oe-mail na sua caixa de entrada, consulte a pasta de spam. O remetente énoreply@edreams.com.     \  Voltar a Iniciar sessão            Ative o Javascript  Para que este site funcione corretamente, tem de ativar o JavaScript</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>https://www.cmjornal.pt</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>https://www.jornaldenegocios.pt</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>https://www.linguee.pt</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>http://www.idealista.pt</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>https://www.legendasdivx.pt</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">									Ligue 210 988 616 | 963 828 885 ou envie-nos um e-mail para: geral@atesempre.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>https://www.jn.pt</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>https://www.ulisboa.pt</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>http://www.acesso.gov.pt</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>E reitoria@ulisboa.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>https://www.ipl.pt</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>https://www.jogossantacasa.pt</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>https://www.lidl.pt</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>https://www.rostos.pt</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>https://www.betclic.pt</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>https://www.iol.pt</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>https://www.observador.pt</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>https://www.elcorteingles.pt</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>https://www.expresso.pt</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>https://www.rtp.pt</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Escolhe esta opção apenas nos teus dispositivos pessoais para manter a tua conta segura.                Iniciar sessão  Já tem uma conta?      Ainda não tem conta? Inscreva-se gratuitamente    Repor a sua palavra-passe  r       Introduza o seu e-mail para receber as instruções para recuperar a palavra-passe:                  Enviar-me as instruções        O e-mail foi enviado para  Siga as instruções no e-mail para repor a sua palavra-passe. Se não receber oe-mail na sua caixa de entrada, consulte a pasta de spam. O remetente énoreply@edreams.com.     \  Voltar a Iniciar sessão            Ative o Javascript  Para que este site funcione corretamente, tem de ativar o JavaScript</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>https://www.cmjornal.pt</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>https://www.jornaldenegocios.pt</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>https://www.linguee.pt</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>http://www.idealista.pt</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>https://www.legendasdivx.pt</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">									Ligue 210 988 616 | 963 828 885 ou envie-nos um e-mail para: geral@atesempre.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>https://www.jn.pt</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>https://www.ulisboa.pt</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>http://www.acesso.gov.pt</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>E reitoria@ulisboa.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>https://www.ipl.pt</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>https://www.jogossantacasa.pt</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>https://www.lidl.pt</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    conta@ipl.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>https://www.rostos.pt</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>https://www.iol.pt</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>https://www.observador.pt</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>https://www.elcorteingles.pt</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>https://www.expresso.pt</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>https://www.cmjornal.pt</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>https://www.jornaldenegocios.pt</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>https://www.jn.pt</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>https://www.ulisboa.pt</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>https://www.ipl.pt</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>https://www.lidl.pt</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>https://www.betclic.pt</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>https://www.shifter.pt</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>https://www.dgsi.pt</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>https://www.castroelectronica.pt</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>https://www.tribunaexpresso.pt</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>https://www.insa.pt</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>https://www.meteo.pt</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>https://www.iapmei.pt</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>https://www.uminho.pt</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>https://www.pousadas.pt</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>http://www.bolanarede.pt</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>https://www.pai.pt</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>https://www.shifter.pt</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>https://www.dgsi.pt</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>https://www.infarmed.pt</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>https://www.shifter.pt</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>https://www.dgsi.pt</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>https://www.castroelectronica.pt</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>http://www.logitravel.pt</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>http://www.imt-ip.pt</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>https://www.castroelectronica.pt</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>http://www.logitravel.pt</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>http://www.imt-ip.pt</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>https://www.castroelectronica.pt</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>https://www.shifter.pt</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>https://www.dgsi.pt</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>https://www.logitravel.pt</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>https://www.imt-ip.pt</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>https://www.shifter.pt</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>https://www.dgsi.pt</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>https://www.castroelectronica.pt</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>https://www.logitravel.pt</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>https://www.imt-ip.pt</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>https://www.expressoemprego.pt</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>http://www.logitravel.pt</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>http://www.imt-ip.pt</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>https://www.sapo.pt</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>http://www.worten.pt</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>https://www.iol.pt</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>https://www.observador.pt</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>http://www.elcorteingles.pt</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>https://www.jornaldenegocios.pt</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>http://www.idealista.pt</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>https://www.jn.pt</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>https://www.ulisboa.pt</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>https://www.ipl.pt</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>https://www.lidl.pt</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>http://www.betclic.pt</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>http://www.pccomponentes.pt</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>https://www.tribunaexpresso.pt</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>http://www.insa.pt</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>http://www.meteo.pt</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>https://www.iapmei.pt</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>https://www.uminho.pt</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>https://www.pousadas.pt</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>http://www.estorilsolcasinos.pt</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>http://www.bolanarede.pt</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>https://www.pai.pt</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>https://www.ipma.pt</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>https://www.publico.pt</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>https://www.dn.pt</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>https://www.uc.pt</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>https://www.novobanco.pt</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>https://www.wook.pt</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>https://www.tsf.pt</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>http://www.mai.gov.pt</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>http://www.tripadvisor.pt</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>https://www.leroymerlin.pt</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>http://www.ul.pt</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>http://www.airbnb.pt</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>https://www.era.pt</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>http://www.pokerstars.pt</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>https://www.proteste.pt</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>http://www.laredoute.pt</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>http://www.motor24.pt</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>https://www.dnoticias.pt</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>http://www.delas.pt</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>http://www.trivago.pt</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>http://www.n-tv.pt</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>http://www.menshealth.pt</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - ?? </t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>https://www.uma.pt</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - YES </t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>